<commit_message>
Fixed issue with Add button not updating current customer.
Fixed issue selecting from unit list not updating current customer.

Fixed selecting between unadded units in unit list not immediately putting them into edit mode
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73961745-8252-4C9E-B049-3A9684975368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16320" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="74">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -252,7 +251,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -739,11 +738,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,20 +1840,24 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="E57" s="13">
+      <c r="D57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="19">
         <v>44136</v>
       </c>
-      <c r="F57" s="11"/>
+      <c r="F57" s="19">
+        <v>44137</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">

</xml_diff>

<commit_message>
Implemented new information for customers and units not in the truck, but only in list.
Print now checks if there are units not in canvas and displays a warning to continue if there is.
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="76">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>When add button is pressed, current customer needs to be changed</t>
+  </si>
+  <si>
+    <t>Implement total units and customers not in canvas</t>
+  </si>
+  <si>
+    <t>OnChange doesn't set editoff</t>
   </si>
 </sst>
 </file>
@@ -742,7 +748,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="F60" sqref="A60:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,38 +1881,64 @@
       <c r="E58" s="19">
         <v>44136</v>
       </c>
-      <c r="F58" s="4"/>
+      <c r="F58" s="19">
+        <v>44137</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="13">
+      <c r="D59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="19">
         <v>44136</v>
       </c>
-      <c r="F59" s="11"/>
+      <c r="F59" s="19">
+        <v>44137</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="6"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
+      <c r="A60" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="19">
+        <v>44137</v>
+      </c>
+      <c r="F60" s="19">
+        <v>44137</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="7"/>
+      <c r="A61" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D61" s="8"/>
-      <c r="E61" s="11"/>
+      <c r="E61" s="13">
+        <v>44137</v>
+      </c>
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed Unit wouldn't stay highlighted as editing in list if also not in canvas.
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -251,7 +251,7 @@
     <t>Implement total units and customers not in canvas</t>
   </si>
   <si>
-    <t>OnChange doesn't set editoff</t>
+    <t>OnChange removes selection of unitList if unit is not in canvas</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F60" sqref="A60:F60"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed rare bug not allowing customers to not be added by forcing customer name to be not a number
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="77">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>OnChange removes selection of unitList if unit is not in canvas</t>
+  </si>
+  <si>
+    <t>Rare bug not allowing customer to be created</t>
   </si>
 </sst>
 </file>
@@ -748,7 +751,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,12 +1945,24 @@
       <c r="F61" s="11"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="6"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
+      <c r="A62" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="19">
+        <v>44138</v>
+      </c>
+      <c r="F62" s="19">
+        <v>44138</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>

</xml_diff>

<commit_message>
Rack is now Customer list, appends -RK if customer is in rack
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="78">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Rare bug not allowing customer to be created</t>
+  </si>
+  <si>
+    <t>When adding only customer to rack, customer says it's not in truck until onChange on customer.</t>
   </si>
 </sst>
 </file>
@@ -750,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,20 +1932,24 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="13">
+      <c r="D61" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="19">
         <v>44137</v>
       </c>
-      <c r="F61" s="11"/>
+      <c r="F61" s="19">
+        <v>44138</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
@@ -1964,12 +1971,20 @@
         <v>44138</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="6"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="7"/>
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D63" s="8"/>
-      <c r="E63" s="11"/>
+      <c r="E63" s="13">
+        <v>44138</v>
+      </c>
       <c r="F63" s="11"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed small issue with customer initially appearing as not in truck when adding only to rack.
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="78">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -754,7 +754,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,11 +1981,15 @@
       <c r="C63" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="8"/>
+      <c r="D63" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="E63" s="13">
         <v>44138</v>
       </c>
-      <c r="F63" s="11"/>
+      <c r="F63" s="13">
+        <v>44138</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>

</xml_diff>

<commit_message>
Added version to scripts on load to trigger re-caching files
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16320" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1972,22 +1972,22 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D63" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="13">
+      <c r="E63" s="19">
         <v>44138</v>
       </c>
-      <c r="F63" s="13">
+      <c r="F63" s="19">
         <v>44138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed unit list dragging error
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYNC\js-truckwrite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAB2E74-D8BE-4F73-A693-333DDEE7EEC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6900"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="81">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -258,12 +259,21 @@
   </si>
   <si>
     <t>When adding only customer to rack, customer says it's not in truck until onChange on customer.</t>
+  </si>
+  <si>
+    <t>When drag and dropping a unit from unit list, if the unit preview causes the list to shift where the mouse is on a different index of the unit list it'll cause an error for sortable js</t>
+  </si>
+  <si>
+    <t>Loading sometimes doesn't restore trailer text</t>
+  </si>
+  <si>
+    <t>Unit edit button stops working when using straps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -750,11 +760,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,28 +2001,52 @@
         <v>44138</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="7"/>
+    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D64" s="8"/>
-      <c r="E64" s="11"/>
+      <c r="E64" s="13">
+        <v>44142</v>
+      </c>
       <c r="F64" s="11"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="6"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="7"/>
+      <c r="A65" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D65" s="8"/>
-      <c r="E65" s="11"/>
+      <c r="E65" s="13">
+        <v>44142</v>
+      </c>
       <c r="F65" s="11"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="7"/>
+      <c r="A66" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D66" s="8"/>
-      <c r="E66" s="11"/>
+      <c r="E66" s="13">
+        <v>44142</v>
+      </c>
       <c r="F66" s="11"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bug fixed: Loading a file with a trailer manually typed wouldn't reload the trailer text
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAB2E74-D8BE-4F73-A693-333DDEE7EEC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="81">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -273,7 +272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -760,11 +759,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,52 +2001,64 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="13">
+      <c r="D64" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="19">
         <v>44142</v>
       </c>
-      <c r="F64" s="11"/>
+      <c r="F64" s="19">
+        <v>44142</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="13">
+      <c r="D65" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="19">
         <v>44142</v>
       </c>
-      <c r="F65" s="11"/>
+      <c r="F65" s="19">
+        <v>44142</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D66" s="8"/>
-      <c r="E66" s="13">
+      <c r="D66" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="19">
         <v>44142</v>
       </c>
-      <c r="F66" s="11"/>
+      <c r="F66" s="19">
+        <v>44142</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>

</xml_diff>

<commit_message>
Fixed preview not working on chrome
Fixed printing not showing height count
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYNC\js-truckwrite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EA8EE1-02D5-42F6-9BE9-C359D9F05449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="82">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -267,12 +268,15 @@
   </si>
   <si>
     <t>Unit edit button stops working when using straps</t>
+  </si>
+  <si>
+    <t>Changing drop sequence doesn't work</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -759,11 +763,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,11 +2065,19 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="7"/>
+      <c r="A67" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D67" s="8"/>
-      <c r="E67" s="11"/>
+      <c r="E67" s="13">
+        <v>44143</v>
+      </c>
       <c r="F67" s="11"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed weight not counting properly on unit updating
Fixed extra text appearing on bottom of canvas
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EA8EE1-02D5-42F6-9BE9-C359D9F05449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E77AA27-AABF-4DEA-AD7E-5EBBDE5013C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="83">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -270,7 +270,10 @@
     <t>Unit edit button stops working when using straps</t>
   </si>
   <si>
-    <t>Changing drop sequence doesn't work</t>
+    <t>Update unit only adds to weight and not removes previous weight</t>
+  </si>
+  <si>
+    <t>Changelog div text appears on webpage sometimes</t>
   </si>
 </sst>
 </file>
@@ -766,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,29 +2067,45 @@
         <v>44142</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B67" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" s="7" t="s">
+      <c r="B67" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="13">
-        <v>44143</v>
-      </c>
-      <c r="F67" s="11"/>
+      <c r="D67" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="19">
+        <v>44170</v>
+      </c>
+      <c r="F67" s="19">
+        <v>44170</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
+      <c r="A68" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="19">
+        <v>44180</v>
+      </c>
+      <c r="F68" s="19">
+        <v>44170</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>

</xml_diff>

<commit_message>
Added load number barcode
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E77AA27-AABF-4DEA-AD7E-5EBBDE5013C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E9A0EF-5E82-4E2F-8516-E3D12D3FCC02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="85">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>Changelog div text appears on webpage sometimes</t>
+  </si>
+  <si>
+    <t>Implement a barcode feature for turckID scanning</t>
+  </si>
+  <si>
+    <t>Tools sometimes unselectable and doesn't add to weight after changing truck</t>
   </si>
 </sst>
 </file>
@@ -769,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2101,26 +2107,42 @@
         <v>9</v>
       </c>
       <c r="E68" s="19">
-        <v>44180</v>
+        <v>44170</v>
       </c>
       <c r="F68" s="19">
         <v>44170</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="7"/>
+      <c r="A69" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D69" s="8"/>
-      <c r="E69" s="11"/>
+      <c r="E69" s="13">
+        <v>44171</v>
+      </c>
       <c r="F69" s="11"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="7"/>
+    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D70" s="8"/>
-      <c r="E70" s="11"/>
+      <c r="E70" s="13">
+        <v>44171</v>
+      </c>
       <c r="F70" s="11"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added locations to queries through GET location parameter
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E9A0EF-5E82-4E2F-8516-E3D12D3FCC02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD5AAF1-3269-41E6-9B1A-0790A91FBD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="86">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Tools sometimes unselectable and doesn't add to weight after changing truck</t>
+  </si>
+  <si>
+    <t>Update changes font size</t>
   </si>
 </sst>
 </file>
@@ -776,7 +779,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2149,9 @@
       <c r="F70" s="11"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
+      <c r="A71" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="B71" s="9"/>
       <c r="C71" s="7"/>
       <c r="D71" s="8"/>

</xml_diff>

<commit_message>
Fixed empty truck dialog
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD5AAF1-3269-41E6-9B1A-0790A91FBD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481EEBE2-9F9F-4208-BD5E-694AD9E36409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="88">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>Update changes font size</t>
+  </si>
+  <si>
+    <t>Importing trucks can be duplicated if truckid has different trucks in it</t>
+  </si>
+  <si>
+    <t>When printing with a weight that is zero, the weight text doesn’t reappear</t>
   </si>
 </sst>
 </file>
@@ -779,7 +785,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+      <selection activeCell="A75" sqref="A74:A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,16 +2164,20 @@
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="6"/>
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="B72" s="9"/>
       <c r="C72" s="7"/>
       <c r="D72" s="8"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
+    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="B73" s="9"/>
       <c r="C73" s="7"/>
       <c r="D73" s="8"/>

</xml_diff>

<commit_message>
FBundles with numbers in type (Bundle 20") no longer imported as units
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481EEBE2-9F9F-4208-BD5E-694AD9E36409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3188AFDB-298E-403E-8580-F8E81846663A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="90">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -282,13 +282,19 @@
     <t>Tools sometimes unselectable and doesn't add to weight after changing truck</t>
   </si>
   <si>
-    <t>Update changes font size</t>
-  </si>
-  <si>
     <t>Importing trucks can be duplicated if truckid has different trucks in it</t>
   </si>
   <si>
-    <t>When printing with a weight that is zero, the weight text doesn’t reappear</t>
+    <t>If two units end in the same last 4 digits, only one appears regardless of customer/drop</t>
+  </si>
+  <si>
+    <t>When loading a save, weight doesn’t show</t>
+  </si>
+  <si>
+    <t>Bundles that have numbers in it show up as units (Bundle 20")</t>
+  </si>
+  <si>
+    <t>Update changes customer font size</t>
   </si>
 </sst>
 </file>
@@ -785,7 +791,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A75" sqref="A74:A75"/>
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,82 +2129,132 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D69" s="8"/>
-      <c r="E69" s="13">
+      <c r="D69" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="19">
         <v>44171</v>
       </c>
-      <c r="F69" s="11"/>
+      <c r="F69" s="19">
+        <v>44171</v>
+      </c>
     </row>
     <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="7" t="s">
+      <c r="B70" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D70" s="8"/>
-      <c r="E70" s="13">
+      <c r="D70" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="19">
         <v>44171</v>
       </c>
-      <c r="F70" s="11"/>
+      <c r="F70" s="19">
+        <v>44171</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B71" s="9"/>
-      <c r="C71" s="7"/>
+        <v>89</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D71" s="8"/>
-      <c r="E71" s="11"/>
+      <c r="E71" s="13">
+        <v>44185</v>
+      </c>
       <c r="F71" s="11"/>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" s="8"/>
+      <c r="E72" s="13">
+        <v>44185</v>
+      </c>
+      <c r="F72" s="11"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="19">
+        <v>44185</v>
+      </c>
+      <c r="F73" s="19">
+        <v>44185</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-    </row>
-    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B73" s="9"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="6"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="7"/>
+      <c r="B74" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D74" s="8"/>
-      <c r="E74" s="11"/>
+      <c r="E74" s="13">
+        <v>44185</v>
+      </c>
       <c r="F74" s="11"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="6"/>
-      <c r="B75" s="9"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
+      <c r="A75" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="19">
+        <v>44185</v>
+      </c>
+      <c r="F75" s="19">
+        <v>44185</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>

</xml_diff>

<commit_message>
Fixed: Selecting a 2 section trucks then a 3 section trucks cause weight text to be placed wrong
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BC4E01-4CAB-47B2-AECC-8EDE1B37CAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="92">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -298,12 +297,15 @@
   </si>
   <si>
     <t>Restoring from save causes weight regions to be placed wrong</t>
+  </si>
+  <si>
+    <t>Selecting 2 section trucks then 3 section trucks cause weight text to be placed wrong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -790,11 +792,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,13 +2277,25 @@
       </c>
       <c r="F76" s="11"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="6"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="19">
+        <v>44194</v>
+      </c>
+      <c r="F77" s="19">
+        <v>44194</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>

</xml_diff>

<commit_message>
Restoring from save causes weight regions to be placed wrong
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="92">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -284,9 +284,6 @@
     <t>Importing trucks can be duplicated if truckid has different trucks in it</t>
   </si>
   <si>
-    <t>If two units end in the same last 4 digits, only one appears regardless of customer/drop</t>
-  </si>
-  <si>
     <t>When loading a save, weight doesn’t show</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>Selecting 2 section trucks then 3 section trucks cause weight text to be placed wrong</t>
+  </si>
+  <si>
+    <t>If two units end in the same last 4 digits during import, only one appears regardless of customer/drop</t>
   </si>
 </sst>
 </file>
@@ -796,7 +796,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>16</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>16</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>16</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>16</v>
@@ -2262,24 +2262,28 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C76" s="7" t="s">
+      <c r="A76" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D76" s="8"/>
-      <c r="E76" s="13">
+      <c r="D76" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="19">
         <v>44185</v>
       </c>
-      <c r="F76" s="11"/>
+      <c r="F76" s="19">
+        <v>44195</v>
+      </c>
     </row>
     <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Fixed bug: Updating units would change name to main customer name if customer has multiple names
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYNC\js-truckwrite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896ED65A-47FC-44AE-B1A8-50A0CF05929F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="97">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -306,12 +307,21 @@
   </si>
   <si>
     <t>Implement Jsdoc</t>
+  </si>
+  <si>
+    <t>Rack toggle doesn’t work if toggling imported home depot with different names</t>
+  </si>
+  <si>
+    <t>Selecting unit from list should remove any search text</t>
+  </si>
+  <si>
+    <t>Add drop down for all customer names</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -809,11 +819,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,24 +2346,46 @@
       </c>
       <c r="F78" s="11"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="6"/>
-      <c r="B79" s="9"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="19">
+        <v>44205</v>
+      </c>
+      <c r="F79" s="19">
+        <v>44205</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="6"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="7"/>
+      <c r="A80" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D80" s="8"/>
-      <c r="E80" s="11"/>
+      <c r="E80" s="13">
+        <v>44205</v>
+      </c>
       <c r="F80" s="11"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="6"/>
+      <c r="A81" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="B81" s="9"/>
       <c r="C81" s="7"/>
       <c r="D81" s="8"/>

</xml_diff>

<commit_message>
Fixed bug: More jsdocs
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896ED65A-47FC-44AE-B1A8-50A0CF05929F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C08D8-549B-4418-9E91-2C235A461D5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="98">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>Add drop down for all customer names</t>
+  </si>
+  <si>
+    <t>Can't update unit twice, possibly because it is the only unit with that name (home depot)</t>
   </si>
 </sst>
 </file>
@@ -823,7 +826,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,20 +2370,24 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B80" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C80" s="7" t="s">
+      <c r="B80" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="13">
+      <c r="D80" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="19">
         <v>44205</v>
       </c>
-      <c r="F80" s="11"/>
+      <c r="F80" s="19">
+        <v>44205</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
@@ -2392,10 +2399,16 @@
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="6"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="7"/>
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D82" s="8"/>
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>

</xml_diff>

<commit_message>
JSDOCS fully implemented for functions
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C08D8-549B-4418-9E91-2C235A461D5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854F4DE0-5678-4D83-8C8D-516CAB0534C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="98">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F82" sqref="A82:F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,18 +2400,24 @@
       <c r="F81" s="11"/>
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B82" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C82" s="7" t="s">
+      <c r="B82" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D82" s="8"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
+      <c r="D82" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="19">
+        <v>44205</v>
+      </c>
+      <c r="F82" s="19">
+        <v>44205</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>

</xml_diff>

<commit_message>
Row information moved to php/server side
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854F4DE0-5678-4D83-8C8D-516CAB0534C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F74186-B758-4A4C-BC7C-9A88C7C77CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="101">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -319,6 +319,15 @@
   </si>
   <si>
     <t>Can't update unit twice, possibly because it is the only unit with that name (home depot)</t>
+  </si>
+  <si>
+    <t>Make the main customer name HD if they are home depots</t>
+  </si>
+  <si>
+    <t>Move rows information to php server side</t>
+  </si>
+  <si>
+    <t>Security</t>
   </si>
 </sst>
 </file>
@@ -825,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F82" sqref="A82:F82"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,20 +2213,24 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B71" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C71" s="7" t="s">
+      <c r="B71" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D71" s="8"/>
-      <c r="E71" s="13">
+      <c r="D71" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="19">
         <v>44185</v>
       </c>
-      <c r="F71" s="11"/>
+      <c r="F71" s="19">
+        <v>44198</v>
+      </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
@@ -2420,7 +2433,9 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="6"/>
+      <c r="A83" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="B83" s="9"/>
       <c r="C83" s="7"/>
       <c r="D83" s="8"/>
@@ -2428,11 +2443,19 @@
       <c r="F83" s="11"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="7"/>
+      <c r="A84" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D84" s="8"/>
-      <c r="E84" s="11"/>
+      <c r="E84" s="13">
+        <v>44206</v>
+      </c>
       <c r="F84" s="11"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed bug Not allowing duplicated units if customer and tag was the same
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F74186-B758-4A4C-BC7C-9A88C7C77CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="103">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -328,12 +327,18 @@
   </si>
   <si>
     <t>Security</t>
+  </si>
+  <si>
+    <t>Cant move both units that have the same last tag numbers to canvas</t>
+  </si>
+  <si>
+    <t>When selecting a unit in unit list that has two of the same customer and last 4 digits it only selects the first one regardless of which you select</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -831,11 +836,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,18 +2463,30 @@
       </c>
       <c r="F84" s="11"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="6"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="7"/>
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D85" s="8"/>
       <c r="E85" s="11"/>
       <c r="F85" s="11"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="6"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="7"/>
+    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D86" s="8"/>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>

</xml_diff>

<commit_message>
Location is now enabled
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SYNC\js-truckwrite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3964EB-768B-42D2-ACFB-3CD653D214E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="104">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -333,12 +334,15 @@
   </si>
   <si>
     <t>When selecting a unit in unit list that has two of the same customer and last 4 digits it only selects the first one regardless of which you select</t>
+  </si>
+  <si>
+    <t>Can't import twice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -836,10 +840,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
       <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
@@ -2492,9 +2496,15 @@
       <c r="F86" s="11"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="6"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="7"/>
+      <c r="A87" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D87" s="8"/>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>

</xml_diff>

<commit_message>
Keep in bounds fixed
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3964EB-768B-42D2-ACFB-3CD653D214E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F47EF5-4161-4841-9084-016590A620DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="105">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>Can't import twice</t>
+  </si>
+  <si>
+    <t>Objects moving away from right side if touching right side of canvas</t>
   </si>
 </sst>
 </file>
@@ -843,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,10 +2512,16 @@
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="6"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="7"/>
+    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D88" s="8"/>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>

</xml_diff>

<commit_message>
Added feature: Option to toggle location unit text on or off
</commit_message>
<xml_diff>
--- a/Bug List.xlsx
+++ b/Bug List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYNC\js-truckwrite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F47EF5-4161-4841-9084-016590A620DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951E804B-C634-41D4-89CD-8ECC3DFEC272}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="104">
   <si>
     <t>Update does not resize text</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>If two units end in the same last 4 digits during import, only one appears regardless of customer/drop</t>
-  </si>
-  <si>
-    <t>Needs testing</t>
   </si>
   <si>
     <t>Implement Jsdoc</t>
@@ -355,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,12 +431,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -468,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -511,11 +502,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,7 +833,7 @@
   <dimension ref="A1:F370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,22 +2267,24 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="26" t="s">
+      <c r="A74" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B74" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C74" s="27" t="s">
+      <c r="B74" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D74" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E74" s="28">
+      <c r="D74" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="19">
         <v>44185</v>
       </c>
-      <c r="F74" s="27"/>
+      <c r="F74" s="19">
+        <v>44208</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
@@ -2360,7 +2348,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>20</v>
@@ -2376,7 +2364,7 @@
     </row>
     <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>16</v>
@@ -2396,7 +2384,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>16</v>
@@ -2416,7 +2404,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B81" s="9"/>
       <c r="C81" s="7"/>
@@ -2426,7 +2414,7 @@
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>16</v>
@@ -2446,7 +2434,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B83" s="9"/>
       <c r="C83" s="7"/>
@@ -2455,76 +2443,104 @@
       <c r="F83" s="11"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B84" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="C84" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E84" s="19">
+        <v>44206</v>
+      </c>
+      <c r="F84" s="19">
+        <v>44208</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C84" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D84" s="8"/>
-      <c r="E84" s="13">
-        <v>44206</v>
-      </c>
-      <c r="F84" s="11"/>
-    </row>
-    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
+      <c r="B85" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="19">
+        <v>44208</v>
+      </c>
+      <c r="F85" s="19">
+        <v>44209</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B85" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C85" s="7" t="s">
+      <c r="B86" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="8"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-    </row>
-    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
+      <c r="D86" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="19">
+        <v>44208</v>
+      </c>
+      <c r="F86" s="19">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B86" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C86" s="7" t="s">
+      <c r="B87" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D86" s="8"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+      <c r="D87" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="19">
+        <v>44211</v>
+      </c>
+      <c r="F87" s="19">
+        <v>44212</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B87" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C87" s="7" t="s">
+      <c r="B88" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D87" s="8"/>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
-    </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D88" s="8"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
+      <c r="D88" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="19">
+        <v>44212</v>
+      </c>
+      <c r="F88" s="19">
+        <v>44213</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>

</xml_diff>